<commit_message>
Endpoints renombrados y código optimizado
</commit_message>
<xml_diff>
--- a/src/utils/trajectories_10133_2008-02-04.xlsx
+++ b/src/utils/trajectories_10133_2008-02-04.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="240" count="240">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="222" count="222">
   <x:si>
     <x:t>taxi_id</x:t>
   </x:si>
@@ -31,709 +31,655 @@
     <x:t>id</x:t>
   </x:si>
   <x:si>
-    <x:t>Sun Feb 03 2008 19:33:38 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 19:03:29 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:01:52 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 19:43:41 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 19:53:44 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 19:23:35 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:13:51 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:03:48 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 19:33:38 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 19:13:32 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:06:54 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:23:54 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:53:10 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:36:54 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:23:20 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:03:13 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:32:51 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:33:22 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:13:16 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:31:26 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:18:34 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 20:33:58 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 23:25:00 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:13:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:36:27 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:46:31 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 21:43:25 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 23:45:05 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 23:52:32 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:11:26 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:02:02 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:07:04 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 23:35:02 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:46:39 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:21:30 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:50:41 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 23:57:34 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Feb 03 2008 23:55:09 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:21:15 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:15:15 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:45:39 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:19:02 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:16:14 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:05:12 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:29:06 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:31:19 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:31:19 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:36:20 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 02:42:45 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 00:16:28 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 02:37:44 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 02:46:21 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 07:55:42 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:42:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:00:43 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 02:44:37 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 07:59:31 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:09:34 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:30:53 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:39:44 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:05:45 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:19:37 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:15:48 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:49:47 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:10:47 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:51:00 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:25:52 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:35:55 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:29:41 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 01:26:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:56:02 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:20:50 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:09:54 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:47:51 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:13:18 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:37:47 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:00:10 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:30:01 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:59:51 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:08:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:56:02 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:40:04 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:03:18 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:28:11 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:03:15 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:32:34 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:50:07 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:32:34 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 09:42:49 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:42:38 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:00:43 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:45:58 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:10:46 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:52:41 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:48:35 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:12:48 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:20:50 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:43:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:25:51 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:15:48 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:02:44 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 10:38:32 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 08:40:57 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:05:45 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:25:51 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:30:53 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:32:54 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:48:35 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:42:58 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:58:38 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:53:01 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:40:05 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:37:21 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:08:41 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:28:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 11:53:36 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:03:40 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:03:04 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:47:24 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:28:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:13:09 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:33:35 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:43:38 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:57:27 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:48:40 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:07:30 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:17:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:38:37 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:16:29 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 12:18:15 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:11:27 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:06:26 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:36:36 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:01:24 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:27:36 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:26:32 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:21:31 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:51:10 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:37:40 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:47:43 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:56:12 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:21:53 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:38:00 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:26:54 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:17:53 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:08:10 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:27:56 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:56:13 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:07:50 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:57:46 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:48:03 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:01:15 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:36:06 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:41:08 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:06:16 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:46:10 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:58:06 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:08:10 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:48:23 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 13:31:34 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 14:51:11 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:21:21 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:38:20 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:16:20 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:18:13 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:26:23 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:46:29 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:11:18 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:51:31 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:08:29 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:41:28 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:58:26 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:36:26 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:06:36 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:56:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:28:36 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:16:39 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:11:38 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:18:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:51:51 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:56:53 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:38:39 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:36:46 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:21:41 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:41:48 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:01:34 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 15:56:33 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:31:44 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:48:43 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:26:43 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:46:49 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:01:54 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:11:58 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:18:53 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:06:56 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:08:49 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:22:01 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 16:58:46 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:27:03 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:37:05 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:32:03 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:16:59 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:28:55 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:38:58 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:42:07 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:47:08 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:49:02 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:52:10 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:07:15 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:57:12 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:19:12 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:17:18 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 17:59:05 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:02:13 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:02:13 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:44:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:09:08 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:29:15 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:49:21 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:59:22 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:12:17 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:39:18 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:22:20 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:59:25 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:54:20 GMT-0500 (hora estándar de Perú)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Feb 04 2008 18:49:19 GMT-0500 (hora estándar de Perú)</x:t>
+    <x:t>2008-02-04T00:33:38.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T00:03:29.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:01:52.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T00:43:41.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T00:53:44.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T00:23:35.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:13:51.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:03:48.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T00:13:32.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:06:54.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:23:54.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:53:10.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:36:54.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:23:20.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:03:13.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:32:51.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:33:22.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:13:16.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:31:26.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:18:34.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T01:33:58.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T04:25:00.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:13:33.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:36:27.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:46:31.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T02:43:25.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T04:45:05.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T04:52:32.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:11:26.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:02:02.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:07:04.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T04:35:02.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:46:39.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:21:30.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:50:41.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T04:57:34.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T04:55:09.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:21:15.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:15:15.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:45:39.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:19:02.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:16:14.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:05:12.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:29:06.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:31:19.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:42:17.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:36:20.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T07:42:45.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T05:16:28.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T07:37:44.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T07:46:21.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T12:55:42.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:00:43.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T07:44:37.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T12:59:31.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:09:34.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:30:53.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:39:44.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:05:45.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:19:37.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:15:48.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:49:47.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:10:47.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:51:00.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:25:52.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:35:55.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:29:41.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T06:26:17.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:56:02.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:20:50.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:09:54.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:47:51.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:13:18.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:37:47.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:00:10.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:30:01.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:59:51.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:08:17.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:40:04.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:03:18.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:28:11.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:03:15.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:32:34.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:50:07.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T14:42:49.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:42:38.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:00:43.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:45:58.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:10:46.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:52:41.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:48:35.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:12:48.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:20:50.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:43:33.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:25:51.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:15:48.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:02:44.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T15:38:32.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T13:40:57.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:05:45.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:30:53.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:32:54.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:48:35.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:42:58.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:58:38.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:53:01.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:40:05.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:37:21.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:08:41.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:28:33.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T16:53:36.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:03:40.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:03:04.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:47:24.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:13:09.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:33:35.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:43:38.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:57:27.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:48:40.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:07:30.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:17:33.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:38:37.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:16:29.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T17:18:15.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:11:27.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:06:26.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:36:36.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:01:24.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:27:36.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:26:32.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:21:31.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:51:10.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:37:40.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:47:43.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:56:12.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:21:53.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:38:00.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:26:54.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:17:53.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:08:10.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:27:56.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:56:13.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:07:50.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:57:46.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:48:03.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:01:15.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:36:06.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:41:08.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:06:16.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:46:10.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:58:06.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:48:23.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T18:31:34.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T19:51:11.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:21:21.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:38:20.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:16:20.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:18:13.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:26:23.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:46:29.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:11:18.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:51:31.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:08:29.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:41:28.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:58:26.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:36:26.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:06:36.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T20:56:33.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:28:36.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:16:39.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:11:38.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:18:33.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:51:51.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:56:53.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:38:39.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:36:46.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:21:41.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:41:48.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:01:34.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:31:44.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:48:43.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:26:43.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:46:49.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:01:54.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:11:58.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:18:53.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:06:56.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:08:49.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:22:01.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T21:58:46.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:27:03.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:37:05.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:32:03.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:16:59.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:28:55.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:38:58.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:42:07.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:47:08.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:49:02.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:52:10.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:07:15.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:57:12.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:19:12.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:17:18.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T22:59:05.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:02:13.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:44:17.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:09:08.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:29:15.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:49:21.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:59:22.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:12:17.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:39:18.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:22:20.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:59:25.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:54:20.000Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2008-02-04T23:49:19.000Z</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1254,7 +1200,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C10" s="0" t="n">
         <x:v>116.47113</x:v>
@@ -1271,7 +1217,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C11" s="0" t="n">
         <x:v>116.42822</x:v>
@@ -1288,7 +1234,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C12" s="0" t="n">
         <x:v>116.4966</x:v>
@@ -1305,7 +1251,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C13" s="0" t="n">
         <x:v>116.45005</x:v>
@@ -1322,7 +1268,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C14" s="0" t="n">
         <x:v>116.37268</x:v>
@@ -1339,7 +1285,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C15" s="0" t="n">
         <x:v>116.40458</x:v>
@@ -1356,7 +1302,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C16" s="0" t="n">
         <x:v>116.278</x:v>
@@ -1373,7 +1319,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C17" s="0" t="n">
         <x:v>116.34882</x:v>
@@ -1390,7 +1336,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C18" s="0" t="n">
         <x:v>116.41121</x:v>
@@ -1407,7 +1353,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C19" s="0" t="n">
         <x:v>116.2809</x:v>
@@ -1424,7 +1370,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C20" s="0" t="n">
         <x:v>116.29624</x:v>
@@ -1441,7 +1387,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C21" s="0" t="n">
         <x:v>116.27744</x:v>
@@ -1458,7 +1404,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C22" s="0" t="n">
         <x:v>116.28618</x:v>
@@ -1475,7 +1421,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C23" s="0" t="n">
         <x:v>116.40846</x:v>
@@ -1492,7 +1438,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C24" s="0" t="n">
         <x:v>116.33167</x:v>
@@ -1509,7 +1455,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C25" s="0" t="n">
         <x:v>116.29541</x:v>
@@ -1526,7 +1472,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C26" s="0" t="n">
         <x:v>116.28637</x:v>
@@ -1543,7 +1489,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C27" s="0" t="n">
         <x:v>116.2783</x:v>
@@ -1560,7 +1506,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C28" s="0" t="n">
         <x:v>116.2694</x:v>
@@ -1577,7 +1523,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C29" s="0" t="n">
         <x:v>116.46057</x:v>
@@ -1594,7 +1540,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C30" s="0" t="n">
         <x:v>116.5046</x:v>
@@ -1611,7 +1557,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C31" s="0" t="n">
         <x:v>116.47177</x:v>
@@ -1628,7 +1574,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C32" s="0" t="n">
         <x:v>116.50194</x:v>
@@ -1645,7 +1591,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C33" s="0" t="n">
         <x:v>116.48449</x:v>
@@ -1662,7 +1608,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C34" s="0" t="n">
         <x:v>116.39308</x:v>
@@ -1679,7 +1625,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C35" s="0" t="n">
         <x:v>116.30911</x:v>
@@ -1696,7 +1642,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C36" s="0" t="n">
         <x:v>116.42116</x:v>
@@ -1713,7 +1659,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C37" s="0" t="n">
         <x:v>116.2583</x:v>
@@ -1730,7 +1676,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C38" s="0" t="n">
         <x:v>116.49658</x:v>
@@ -1747,7 +1693,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C39" s="0" t="n">
         <x:v>116.50464</x:v>
@@ -1764,7 +1710,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C40" s="0" t="n">
         <x:v>116.14118</x:v>
@@ -1781,7 +1727,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C41" s="0" t="n">
         <x:v>116.46911</x:v>
@@ -1798,7 +1744,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C42" s="0" t="n">
         <x:v>116.31288</x:v>
@@ -1815,7 +1761,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C43" s="0" t="n">
         <x:v>116.14111</x:v>
@@ -1832,7 +1778,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C44" s="0" t="n">
         <x:v>116.14127</x:v>
@@ -1849,7 +1795,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C45" s="0" t="n">
         <x:v>116.49648</x:v>
@@ -1866,7 +1812,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C46" s="0" t="n">
         <x:v>116.14436</x:v>
@@ -1883,7 +1829,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C47" s="0" t="n">
         <x:v>116.14361</x:v>
@@ -1900,7 +1846,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C48" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -1917,7 +1863,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C49" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -1934,7 +1880,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C50" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -1951,7 +1897,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C51" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -1968,7 +1914,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C52" s="0" t="n">
         <x:v>116.14361</x:v>
@@ -1985,7 +1931,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C53" s="0" t="n">
         <x:v>116.14139</x:v>
@@ -2002,7 +1948,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C54" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -2019,7 +1965,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C55" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -2036,7 +1982,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C56" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -2053,7 +1999,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C57" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -2070,7 +2016,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C58" s="0" t="n">
         <x:v>116.14474</x:v>
@@ -2087,7 +2033,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C59" s="0" t="n">
         <x:v>116.46323</x:v>
@@ -2104,7 +2050,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C60" s="0" t="n">
         <x:v>116.14456</x:v>
@@ -2121,7 +2067,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C61" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -2138,7 +2084,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C62" s="0" t="n">
         <x:v>116.15585</x:v>
@@ -2155,7 +2101,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C63" s="0" t="n">
         <x:v>116.16558</x:v>
@@ -2172,7 +2118,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C64" s="0" t="n">
         <x:v>116.14138</x:v>
@@ -2189,7 +2135,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C65" s="0" t="n">
         <x:v>116.16562</x:v>
@@ -2206,7 +2152,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C66" s="0" t="n">
         <x:v>116.15718</x:v>
@@ -2223,7 +2169,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C67" s="0" t="n">
         <x:v>116.16562</x:v>
@@ -2240,7 +2186,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C68" s="0" t="n">
         <x:v>116.16563</x:v>
@@ -2257,7 +2203,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C69" s="0" t="n">
         <x:v>116.13586</x:v>
@@ -2274,7 +2220,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C70" s="0" t="n">
         <x:v>116.19</x:v>
@@ -2291,7 +2237,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C71" s="0" t="n">
         <x:v>116.1656</x:v>
@@ -2308,7 +2254,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C72" s="0" t="n">
         <x:v>116.15831</x:v>
@@ -2325,7 +2271,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C73" s="0" t="n">
         <x:v>116.16151</x:v>
@@ -2342,7 +2288,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C74" s="0" t="n">
         <x:v>116.25857</x:v>
@@ -2359,7 +2305,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C75" s="0" t="n">
         <x:v>116.16561</x:v>
@@ -2376,7 +2322,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C76" s="0" t="n">
         <x:v>116.27261</x:v>
@@ -2393,7 +2339,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C77" s="0" t="n">
         <x:v>116.14375</x:v>
@@ -2410,7 +2356,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C78" s="0" t="n">
         <x:v>116.14062</x:v>
@@ -2427,7 +2373,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C79" s="0" t="n">
         <x:v>116.13585</x:v>
@@ -2444,7 +2390,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C80" s="0" t="n">
         <x:v>116.14362</x:v>
@@ -2461,7 +2407,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C81" s="0" t="n">
         <x:v>116.30151</x:v>
@@ -2478,7 +2424,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C82" s="0" t="n">
         <x:v>116.15296</x:v>
@@ -2495,7 +2441,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C83" s="0" t="n">
         <x:v>116.30646</x:v>
@@ -2512,7 +2458,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C84" s="0" t="n">
         <x:v>116.3468</x:v>
@@ -2529,7 +2475,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C85" s="0" t="n">
         <x:v>116.31342</x:v>
@@ -2546,7 +2492,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C86" s="0" t="n">
         <x:v>116.36498</x:v>
@@ -2563,7 +2509,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C87" s="0" t="n">
         <x:v>116.37777</x:v>
@@ -2580,7 +2526,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C88" s="0" t="n">
         <x:v>116.36817</x:v>
@@ -2597,7 +2543,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C89" s="0" t="n">
         <x:v>116.30253</x:v>
@@ -2614,7 +2560,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C90" s="0" t="n">
         <x:v>116.30519</x:v>
@@ -2631,7 +2577,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C91" s="0" t="n">
         <x:v>116.30151</x:v>
@@ -2648,7 +2594,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C92" s="0" t="n">
         <x:v>116.35584</x:v>
@@ -2665,7 +2611,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C93" s="0" t="n">
         <x:v>116.38698</x:v>
@@ -2682,7 +2628,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C94" s="0" t="n">
         <x:v>116.36791</x:v>
@@ -2699,7 +2645,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C95" s="0" t="n">
         <x:v>116.30457</x:v>
@@ -2716,7 +2662,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C96" s="0" t="n">
         <x:v>116.38094</x:v>
@@ -2733,7 +2679,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C97" s="0" t="n">
         <x:v>116.34688</x:v>
@@ -2750,7 +2696,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C98" s="0" t="n">
         <x:v>116.38094</x:v>
@@ -2767,7 +2713,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B99" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C99" s="0" t="n">
         <x:v>116.34691</x:v>
@@ -2784,7 +2730,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C100" s="0" t="n">
         <x:v>116.39379</x:v>
@@ -2801,7 +2747,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B101" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C101" s="0" t="n">
         <x:v>116.37859</x:v>
@@ -2818,7 +2764,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B102" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C102" s="0" t="n">
         <x:v>116.21926</x:v>
@@ -2835,7 +2781,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B103" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C103" s="0" t="n">
         <x:v>116.37027</x:v>
@@ -2852,7 +2798,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B104" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C104" s="0" t="n">
         <x:v>116.39238</x:v>
@@ -2869,7 +2815,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B105" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C105" s="0" t="n">
         <x:v>116.39296</x:v>
@@ -2886,7 +2832,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B106" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C106" s="0" t="n">
         <x:v>116.36829</x:v>
@@ -2903,7 +2849,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B107" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C107" s="0" t="n">
         <x:v>116.36124</x:v>
@@ -2920,7 +2866,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B108" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C108" s="0" t="n">
         <x:v>116.39399</x:v>
@@ -2937,7 +2883,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B109" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C109" s="0" t="n">
         <x:v>116.35063</x:v>
@@ -2954,7 +2900,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B110" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C110" s="0" t="n">
         <x:v>116.36802</x:v>
@@ -2971,7 +2917,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B111" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="C111" s="0" t="n">
         <x:v>116.37821</x:v>
@@ -2988,7 +2934,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B112" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C112" s="0" t="n">
         <x:v>116.40035</x:v>
@@ -3005,7 +2951,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B113" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="C113" s="0" t="n">
         <x:v>116.19669</x:v>
@@ -3022,7 +2968,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B114" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C114" s="0" t="n">
         <x:v>116.3753</x:v>
@@ -3039,7 +2985,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B115" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C115" s="0" t="n">
         <x:v>116.35063</x:v>
@@ -3056,7 +3002,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B116" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="C116" s="0" t="n">
         <x:v>116.34998</x:v>
@@ -3073,7 +3019,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B117" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C117" s="0" t="n">
         <x:v>116.34974</x:v>
@@ -3090,7 +3036,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B118" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C118" s="0" t="n">
         <x:v>116.37041</x:v>
@@ -3107,7 +3053,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B119" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C119" s="0" t="n">
         <x:v>116.34897</x:v>
@@ -3124,7 +3070,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B120" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="C120" s="0" t="n">
         <x:v>116.3497</x:v>
@@ -3141,7 +3087,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B121" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C121" s="0" t="n">
         <x:v>116.36549</x:v>
@@ -3158,7 +3104,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B122" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C122" s="0" t="n">
         <x:v>116.34934</x:v>
@@ -3175,7 +3121,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B123" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C123" s="0" t="n">
         <x:v>116.31624</x:v>
@@ -3192,7 +3138,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B124" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C124" s="0" t="n">
         <x:v>116.34323</x:v>
@@ -3209,7 +3155,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B125" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C125" s="0" t="n">
         <x:v>116.33817</x:v>
@@ -3226,7 +3172,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B126" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C126" s="0" t="n">
         <x:v>116.36518</x:v>
@@ -3243,7 +3189,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B127" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C127" s="0" t="n">
         <x:v>116.33928</x:v>
@@ -3260,7 +3206,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B128" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C128" s="0" t="n">
         <x:v>116.34215</x:v>
@@ -3277,7 +3223,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B129" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C129" s="0" t="n">
         <x:v>116.30231</x:v>
@@ -3294,7 +3240,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B130" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C130" s="0" t="n">
         <x:v>116.33817</x:v>
@@ -3311,7 +3257,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B131" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="C131" s="0" t="n">
         <x:v>116.34025</x:v>
@@ -3328,7 +3274,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B132" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C132" s="0" t="n">
         <x:v>116.32828</x:v>
@@ -3345,7 +3291,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B133" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="C133" s="0" t="n">
         <x:v>116.3039</x:v>
@@ -3362,7 +3308,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B134" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C134" s="0" t="n">
         <x:v>116.31487</x:v>
@@ -3379,7 +3325,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B135" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C135" s="0" t="n">
         <x:v>116.30395</x:v>
@@ -3396,7 +3342,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B136" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C136" s="0" t="n">
         <x:v>116.31294</x:v>
@@ -3413,7 +3359,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B137" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C137" s="0" t="n">
         <x:v>116.29364</x:v>
@@ -3430,7 +3376,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B138" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C138" s="0" t="n">
         <x:v>116.31445</x:v>
@@ -3447,7 +3393,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B139" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="C139" s="0" t="n">
         <x:v>116.29368</x:v>
@@ -3464,7 +3410,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B140" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C140" s="0" t="n">
         <x:v>116.34025</x:v>
@@ -3481,7 +3427,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B141" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="C141" s="0" t="n">
         <x:v>116.2986</x:v>
@@ -3498,7 +3444,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B142" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="C142" s="0" t="n">
         <x:v>116.31511</x:v>
@@ -3515,7 +3461,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B143" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="C143" s="0" t="n">
         <x:v>116.2968</x:v>
@@ -3532,7 +3478,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B144" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="C144" s="0" t="n">
         <x:v>116.31507</x:v>
@@ -3549,7 +3495,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B145" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="C145" s="0" t="n">
         <x:v>116.29373</x:v>
@@ -3566,7 +3512,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B146" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="C146" s="0" t="n">
         <x:v>116.29373</x:v>
@@ -3583,7 +3529,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B147" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="C147" s="0" t="n">
         <x:v>116.29371</x:v>
@@ -3600,7 +3546,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B148" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="C148" s="0" t="n">
         <x:v>116.31978</x:v>
@@ -3617,7 +3563,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B149" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="C149" s="0" t="n">
         <x:v>116.29676</x:v>
@@ -3634,7 +3580,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B150" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C150" s="0" t="n">
         <x:v>116.30875</x:v>
@@ -3651,7 +3597,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B151" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="C151" s="0" t="n">
         <x:v>116.31485</x:v>
@@ -3668,7 +3614,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B152" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C152" s="0" t="n">
         <x:v>116.20228</x:v>
@@ -3685,7 +3631,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B153" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C153" s="0" t="n">
         <x:v>116.17914</x:v>
@@ -3702,7 +3648,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B154" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C154" s="0" t="n">
         <x:v>116.19824</x:v>
@@ -3719,7 +3665,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B155" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="C155" s="0" t="n">
         <x:v>116.23009</x:v>
@@ -3736,7 +3682,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B156" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C156" s="0" t="n">
         <x:v>116.25437</x:v>
@@ -3753,7 +3699,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B157" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="C157" s="0" t="n">
         <x:v>116.20044</x:v>
@@ -3770,7 +3716,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B158" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C158" s="0" t="n">
         <x:v>116.231</x:v>
@@ -3787,7 +3733,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B159" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="C159" s="0" t="n">
         <x:v>116.26947</x:v>
@@ -3804,7 +3750,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B160" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="C160" s="0" t="n">
         <x:v>116.3053</x:v>
@@ -3821,7 +3767,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B161" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="C161" s="0" t="n">
         <x:v>116.19359</x:v>
@@ -3838,7 +3784,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B162" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="C162" s="0" t="n">
         <x:v>116.25286</x:v>
@@ -3855,7 +3801,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B163" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C163" s="0" t="n">
         <x:v>116.17663</x:v>
@@ -3872,7 +3818,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B164" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="C164" s="0" t="n">
         <x:v>116.18553</x:v>
@@ -3889,7 +3835,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B165" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="C165" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -3906,7 +3852,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B166" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="C166" s="0" t="n">
         <x:v>116.192</x:v>
@@ -3923,7 +3869,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B167" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C167" s="0" t="n">
         <x:v>116.2412</x:v>
@@ -3940,7 +3886,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B168" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C168" s="0" t="n">
         <x:v>116.25437</x:v>
@@ -3957,7 +3903,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B169" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C169" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -3974,7 +3920,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B170" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="C170" s="0" t="n">
         <x:v>116.29367</x:v>
@@ -3991,7 +3937,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B171" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="C171" s="0" t="n">
         <x:v>116.20187</x:v>
@@ -4008,7 +3954,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B172" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="C172" s="0" t="n">
         <x:v>116.25438</x:v>
@@ -4025,7 +3971,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B173" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="C173" s="0" t="n">
         <x:v>116.25445</x:v>
@@ -4042,7 +3988,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B174" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="C174" s="0" t="n">
         <x:v>116.2544</x:v>
@@ -4059,7 +4005,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B175" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="C175" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -4076,7 +4022,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B176" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="C176" s="0" t="n">
         <x:v>116.25438</x:v>
@@ -4093,7 +4039,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B177" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="C177" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -4110,7 +4056,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B178" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="C178" s="0" t="n">
         <x:v>116.25445</x:v>
@@ -4127,7 +4073,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B179" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="C179" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -4144,7 +4090,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B180" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="C180" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -4161,7 +4107,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B181" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="C181" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -4178,7 +4124,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B182" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="C182" s="0" t="n">
         <x:v>116.25445</x:v>
@@ -4195,7 +4141,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B183" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="C183" s="0" t="n">
         <x:v>116.25443</x:v>
@@ -4212,7 +4158,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B184" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C184" s="0" t="n">
         <x:v>116.25441</x:v>
@@ -4229,7 +4175,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B185" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="C185" s="0" t="n">
         <x:v>116.25437</x:v>
@@ -4246,7 +4192,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B186" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="C186" s="0" t="n">
         <x:v>116.25445</x:v>
@@ -4263,7 +4209,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B187" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="C187" s="0" t="n">
         <x:v>116.25443</x:v>
@@ -4280,7 +4226,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B188" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="C188" s="0" t="n">
         <x:v>116.25442</x:v>
@@ -4297,7 +4243,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B189" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="C189" s="0" t="n">
         <x:v>116.25446</x:v>
@@ -4314,7 +4260,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B190" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="C190" s="0" t="n">
         <x:v>116.25441</x:v>
@@ -4331,7 +4277,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B191" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C191" s="0" t="n">
         <x:v>116.25443</x:v>
@@ -4348,7 +4294,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B192" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="C192" s="0" t="n">
         <x:v>116.25443</x:v>
@@ -4365,7 +4311,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B193" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="C193" s="0" t="n">
         <x:v>116.25449</x:v>
@@ -4382,7 +4328,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B194" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="C194" s="0" t="n">
         <x:v>116.25448</x:v>
@@ -4399,7 +4345,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B195" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="C195" s="0" t="n">
         <x:v>116.25438</x:v>
@@ -4416,7 +4362,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B196" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="C196" s="0" t="n">
         <x:v>116.25439</x:v>
@@ -4433,7 +4379,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B197" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="C197" s="0" t="n">
         <x:v>116.25437</x:v>
@@ -4450,7 +4396,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B198" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="C198" s="0" t="n">
         <x:v>116.25438</x:v>
@@ -4467,7 +4413,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B199" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="C199" s="0" t="n">
         <x:v>116.25447</x:v>
@@ -4484,7 +4430,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B200" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="C200" s="0" t="n">
         <x:v>116.25435</x:v>
@@ -4501,7 +4447,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B201" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="C201" s="0" t="n">
         <x:v>116.25437</x:v>
@@ -4518,7 +4464,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B202" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="C202" s="0" t="n">
         <x:v>116.2544</x:v>
@@ -4535,7 +4481,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B203" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="C203" s="0" t="n">
         <x:v>116.25439</x:v>
@@ -4552,7 +4498,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B204" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="C204" s="0" t="n">
         <x:v>116.25434</x:v>
@@ -4569,7 +4515,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B205" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="C205" s="0" t="n">
         <x:v>116.25444</x:v>
@@ -4586,7 +4532,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B206" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="C206" s="0" t="n">
         <x:v>116.25445</x:v>
@@ -4603,7 +4549,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B207" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="C207" s="0" t="n">
         <x:v>116.25434</x:v>
@@ -4620,7 +4566,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B208" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="C208" s="0" t="n">
         <x:v>116.25443</x:v>
@@ -4637,7 +4583,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B209" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="C209" s="0" t="n">
         <x:v>116.25441</x:v>
@@ -4654,7 +4600,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B210" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="C210" s="0" t="n">
         <x:v>116.25446</x:v>
@@ -4671,7 +4617,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B211" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="C211" s="0" t="n">
         <x:v>116.2544</x:v>
@@ -4688,7 +4634,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B212" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C212" s="0" t="n">
         <x:v>116.2544</x:v>
@@ -4705,7 +4651,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B213" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="C213" s="0" t="n">
         <x:v>116.25445</x:v>
@@ -4722,7 +4668,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B214" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="C214" s="0" t="n">
         <x:v>116.25441</x:v>
@@ -4739,7 +4685,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B215" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="C215" s="0" t="n">
         <x:v>116.25439</x:v>
@@ -4756,7 +4702,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B216" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="C216" s="0" t="n">
         <x:v>116.25575</x:v>
@@ -4773,7 +4719,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B217" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="C217" s="0" t="n">
         <x:v>116.25125</x:v>
@@ -4790,7 +4736,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B218" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="C218" s="0" t="n">
         <x:v>116.26015</x:v>
@@ -4807,7 +4753,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B219" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="C219" s="0" t="n">
         <x:v>116.27307</x:v>
@@ -4824,7 +4770,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B220" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="C220" s="0" t="n">
         <x:v>116.26871</x:v>
@@ -4841,7 +4787,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B221" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="C221" s="0" t="n">
         <x:v>116.30389</x:v>
@@ -4858,7 +4804,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B222" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="C222" s="0" t="n">
         <x:v>116.30388</x:v>
@@ -4875,7 +4821,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B223" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="C223" s="0" t="n">
         <x:v>116.26296</x:v>
@@ -4892,7 +4838,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B224" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="C224" s="0" t="n">
         <x:v>116.26798</x:v>
@@ -4909,7 +4855,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B225" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="C225" s="0" t="n">
         <x:v>116.26798</x:v>
@@ -4926,7 +4872,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B226" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="C226" s="0" t="n">
         <x:v>116.36082</x:v>
@@ -4943,7 +4889,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B227" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="C227" s="0" t="n">
         <x:v>116.28219</x:v>
@@ -4960,7 +4906,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B228" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="C228" s="0" t="n">
         <x:v>116.31209</x:v>
@@ -4977,7 +4923,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B229" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="C229" s="0" t="n">
         <x:v>116.35694</x:v>
@@ -4994,7 +4940,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B230" s="0" t="s">
-        <x:v>233</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="C230" s="0" t="n">
         <x:v>116.35705</x:v>
@@ -5011,7 +4957,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B231" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="C231" s="0" t="n">
         <x:v>116.29833</x:v>
@@ -5028,7 +4974,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B232" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="C232" s="0" t="n">
         <x:v>116.357</x:v>
@@ -5045,7 +4991,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B233" s="0" t="s">
-        <x:v>236</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C233" s="0" t="n">
         <x:v>116.30391</x:v>
@@ -5062,7 +5008,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B234" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C234" s="0" t="n">
         <x:v>116.35703</x:v>
@@ -5079,7 +5025,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B235" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="C235" s="0" t="n">
         <x:v>116.35703</x:v>
@@ -5096,7 +5042,7 @@
         <x:v>10133</x:v>
       </x:c>
       <x:c r="B236" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C236" s="0" t="n">
         <x:v>116.35694</x:v>

</xml_diff>